<commit_message>
branch:progressXL Oct2nd Second commit
</commit_message>
<xml_diff>
--- a/ProgressExcel.xlsx
+++ b/ProgressExcel.xlsx
@@ -418,7 +418,7 @@
   <dimension ref="A1:N97"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -504,11 +504,11 @@
         <v>1.5</v>
       </c>
       <c r="D4">
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="N4">
         <f t="shared" ref="N4:N67" si="0">SUM(C4:J4)</f>
-        <v>2.5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
progressXL progressXL updated. Some random file also preset
</commit_message>
<xml_diff>
--- a/ProgressExcel.xlsx
+++ b/ProgressExcel.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="96" yWindow="36" windowWidth="19140" windowHeight="9552"/>
+    <workbookView xWindow="96" yWindow="36" windowWidth="19140" windowHeight="9552" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="21">
   <si>
     <t>Date</t>
   </si>
@@ -37,9 +37,6 @@
   </si>
   <si>
     <t>udemy Java</t>
-  </si>
-  <si>
-    <t>leetcode</t>
   </si>
   <si>
     <t>Java DS and Algos</t>
@@ -67,6 +64,21 @@
   </si>
   <si>
     <t>Maven PluralSight</t>
+  </si>
+  <si>
+    <t>leetcode/interviewbit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">API endpoints Session2 </t>
+  </si>
+  <si>
+    <t>Git Session 1 and Session2</t>
+  </si>
+  <si>
+    <t>leetcode/nterviewBit</t>
+  </si>
+  <si>
+    <t>1 program, running time analysis</t>
   </si>
 </sst>
 </file>
@@ -417,8 +429,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N97"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -462,19 +474,19 @@
         <v>6</v>
       </c>
       <c r="H2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I2" t="s">
         <v>7</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>8</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
+        <v>14</v>
+      </c>
+      <c r="N2" t="s">
         <v>9</v>
-      </c>
-      <c r="K2" t="s">
-        <v>15</v>
-      </c>
-      <c r="N2" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.3">
@@ -506,9 +518,12 @@
       <c r="D4">
         <v>1.5</v>
       </c>
+      <c r="H4">
+        <v>0.5</v>
+      </c>
       <c r="N4">
         <f t="shared" ref="N4:N67" si="0">SUM(C4:J4)</f>
-        <v>3</v>
+        <v>3.5</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.3">
@@ -1430,8 +1445,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J97"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="18.6640625" defaultRowHeight="34.200000000000003" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1443,7 +1458,7 @@
   <sheetData>
     <row r="1" spans="1:10" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B1" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
@@ -1466,16 +1481,16 @@
         <v>6</v>
       </c>
       <c r="G2" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="I2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="I2" s="2" t="s">
-        <v>9</v>
-      </c>
       <c r="J2" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
@@ -1483,19 +1498,28 @@
         <v>43739</v>
       </c>
       <c r="B3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="E3" s="2" t="s">
         <v>13</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="3">
         <f>A3+1</f>
         <v>43740</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Updated for Oct 3rd
</commit_message>
<xml_diff>
--- a/ProgressExcel.xlsx
+++ b/ProgressExcel.xlsx
@@ -1,17 +1,31 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Anil\Courses\progressXL\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3042E85-20BA-4861-8123-1CFED0E49645}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="96" yWindow="36" windowWidth="19140" windowHeight="9552" activeTab="1"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -84,10 +98,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="d\-mmm\-yy"/>
-  </numFmts>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -119,11 +130,11 @@
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -135,6 +146,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -183,7 +197,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -216,9 +230,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -251,6 +282,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -426,35 +474,35 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N97"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.21875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.21875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.44140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.44140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.44140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="4.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="4.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -489,7 +537,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>43739</v>
       </c>
@@ -507,7 +555,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <f>A3+1</f>
         <v>43740</v>
@@ -526,17 +574,32 @@
         <v>3.5</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <f t="shared" ref="A5:A68" si="1">A4+1</f>
         <v>43741</v>
       </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
       <c r="N5">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <f t="shared" si="1"/>
         <v>43742</v>
@@ -546,7 +609,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <f t="shared" si="1"/>
         <v>43743</v>
@@ -556,7 +619,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <f t="shared" si="1"/>
         <v>43744</v>
@@ -566,7 +629,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <f t="shared" si="1"/>
         <v>43745</v>
@@ -576,7 +639,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <f t="shared" si="1"/>
         <v>43746</v>
@@ -586,7 +649,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <f t="shared" si="1"/>
         <v>43747</v>
@@ -596,7 +659,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <f t="shared" si="1"/>
         <v>43748</v>
@@ -606,7 +669,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <f t="shared" si="1"/>
         <v>43749</v>
@@ -616,7 +679,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <f t="shared" si="1"/>
         <v>43750</v>
@@ -626,7 +689,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <f t="shared" si="1"/>
         <v>43751</v>
@@ -636,7 +699,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <f t="shared" si="1"/>
         <v>43752</v>
@@ -646,7 +709,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <f t="shared" si="1"/>
         <v>43753</v>
@@ -656,7 +719,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <f t="shared" si="1"/>
         <v>43754</v>
@@ -666,7 +729,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <f t="shared" si="1"/>
         <v>43755</v>
@@ -676,7 +739,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <f t="shared" si="1"/>
         <v>43756</v>
@@ -686,7 +749,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <f t="shared" si="1"/>
         <v>43757</v>
@@ -696,7 +759,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <f t="shared" si="1"/>
         <v>43758</v>
@@ -706,7 +769,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <f t="shared" si="1"/>
         <v>43759</v>
@@ -716,7 +779,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <f t="shared" si="1"/>
         <v>43760</v>
@@ -726,7 +789,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <f t="shared" si="1"/>
         <v>43761</v>
@@ -736,7 +799,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <f t="shared" si="1"/>
         <v>43762</v>
@@ -746,7 +809,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <f t="shared" si="1"/>
         <v>43763</v>
@@ -756,7 +819,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <f t="shared" si="1"/>
         <v>43764</v>
@@ -766,7 +829,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <f t="shared" si="1"/>
         <v>43765</v>
@@ -776,7 +839,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <f t="shared" si="1"/>
         <v>43766</v>
@@ -786,7 +849,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <f t="shared" si="1"/>
         <v>43767</v>
@@ -796,7 +859,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <f t="shared" si="1"/>
         <v>43768</v>
@@ -806,7 +869,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <f t="shared" si="1"/>
         <v>43769</v>
@@ -816,7 +879,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <f t="shared" si="1"/>
         <v>43770</v>
@@ -826,7 +889,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <f t="shared" si="1"/>
         <v>43771</v>
@@ -836,7 +899,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <f t="shared" si="1"/>
         <v>43772</v>
@@ -846,7 +909,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <f t="shared" si="1"/>
         <v>43773</v>
@@ -856,7 +919,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <f t="shared" si="1"/>
         <v>43774</v>
@@ -866,7 +929,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <f t="shared" si="1"/>
         <v>43775</v>
@@ -876,7 +939,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <f t="shared" si="1"/>
         <v>43776</v>
@@ -886,7 +949,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <f t="shared" si="1"/>
         <v>43777</v>
@@ -896,7 +959,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
         <f t="shared" si="1"/>
         <v>43778</v>
@@ -906,7 +969,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
         <f t="shared" si="1"/>
         <v>43779</v>
@@ -916,7 +979,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
         <f t="shared" si="1"/>
         <v>43780</v>
@@ -926,7 +989,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
         <f t="shared" si="1"/>
         <v>43781</v>
@@ -936,7 +999,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
         <f t="shared" si="1"/>
         <v>43782</v>
@@ -946,7 +1009,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
         <f t="shared" si="1"/>
         <v>43783</v>
@@ -956,7 +1019,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
         <f t="shared" si="1"/>
         <v>43784</v>
@@ -966,7 +1029,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
         <f t="shared" si="1"/>
         <v>43785</v>
@@ -976,7 +1039,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
         <f t="shared" si="1"/>
         <v>43786</v>
@@ -986,7 +1049,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
         <f t="shared" si="1"/>
         <v>43787</v>
@@ -996,7 +1059,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A52" s="1">
         <f t="shared" si="1"/>
         <v>43788</v>
@@ -1006,7 +1069,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A53" s="1">
         <f t="shared" si="1"/>
         <v>43789</v>
@@ -1016,7 +1079,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A54" s="1">
         <f t="shared" si="1"/>
         <v>43790</v>
@@ -1026,7 +1089,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A55" s="1">
         <f t="shared" si="1"/>
         <v>43791</v>
@@ -1036,7 +1099,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A56" s="1">
         <f t="shared" si="1"/>
         <v>43792</v>
@@ -1046,7 +1109,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A57" s="1">
         <f t="shared" si="1"/>
         <v>43793</v>
@@ -1056,7 +1119,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A58" s="1">
         <f t="shared" si="1"/>
         <v>43794</v>
@@ -1066,7 +1129,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A59" s="1">
         <f t="shared" si="1"/>
         <v>43795</v>
@@ -1076,7 +1139,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A60" s="1">
         <f t="shared" si="1"/>
         <v>43796</v>
@@ -1086,7 +1149,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A61" s="1">
         <f t="shared" si="1"/>
         <v>43797</v>
@@ -1096,7 +1159,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A62" s="1">
         <f t="shared" si="1"/>
         <v>43798</v>
@@ -1106,7 +1169,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A63" s="1">
         <f t="shared" si="1"/>
         <v>43799</v>
@@ -1116,7 +1179,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A64" s="1">
         <f t="shared" si="1"/>
         <v>43800</v>
@@ -1126,7 +1189,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A65" s="1">
         <f t="shared" si="1"/>
         <v>43801</v>
@@ -1136,7 +1199,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A66" s="1">
         <f t="shared" si="1"/>
         <v>43802</v>
@@ -1146,7 +1209,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A67" s="1">
         <f t="shared" si="1"/>
         <v>43803</v>
@@ -1156,7 +1219,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A68" s="1">
         <f t="shared" si="1"/>
         <v>43804</v>
@@ -1166,7 +1229,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A69" s="1">
         <f t="shared" ref="A69:A94" si="3">A68+1</f>
         <v>43805</v>
@@ -1176,7 +1239,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A70" s="1">
         <f t="shared" si="3"/>
         <v>43806</v>
@@ -1186,7 +1249,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A71" s="1">
         <f t="shared" si="3"/>
         <v>43807</v>
@@ -1196,7 +1259,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A72" s="1">
         <f t="shared" si="3"/>
         <v>43808</v>
@@ -1206,7 +1269,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A73" s="1">
         <f t="shared" si="3"/>
         <v>43809</v>
@@ -1216,7 +1279,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A74" s="1">
         <f t="shared" si="3"/>
         <v>43810</v>
@@ -1226,7 +1289,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A75" s="1">
         <f t="shared" si="3"/>
         <v>43811</v>
@@ -1236,7 +1299,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A76" s="1">
         <f t="shared" si="3"/>
         <v>43812</v>
@@ -1246,7 +1309,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A77" s="1">
         <f t="shared" si="3"/>
         <v>43813</v>
@@ -1256,7 +1319,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A78" s="1">
         <f t="shared" si="3"/>
         <v>43814</v>
@@ -1266,7 +1329,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A79" s="1">
         <f t="shared" si="3"/>
         <v>43815</v>
@@ -1276,7 +1339,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A80" s="1">
         <f t="shared" si="3"/>
         <v>43816</v>
@@ -1286,7 +1349,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A81" s="1">
         <f t="shared" si="3"/>
         <v>43817</v>
@@ -1296,7 +1359,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A82" s="1">
         <f t="shared" si="3"/>
         <v>43818</v>
@@ -1306,7 +1369,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A83" s="1">
         <f t="shared" si="3"/>
         <v>43819</v>
@@ -1316,7 +1379,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A84" s="1">
         <f t="shared" si="3"/>
         <v>43820</v>
@@ -1326,7 +1389,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A85" s="1">
         <f t="shared" si="3"/>
         <v>43821</v>
@@ -1336,7 +1399,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A86" s="1">
         <f t="shared" si="3"/>
         <v>43822</v>
@@ -1346,7 +1409,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A87" s="1">
         <f t="shared" si="3"/>
         <v>43823</v>
@@ -1356,7 +1419,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A88" s="1">
         <f t="shared" si="3"/>
         <v>43824</v>
@@ -1366,7 +1429,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A89" s="1">
         <f t="shared" si="3"/>
         <v>43825</v>
@@ -1376,7 +1439,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A90" s="1">
         <f t="shared" si="3"/>
         <v>43826</v>
@@ -1386,7 +1449,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="91" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A91" s="1">
         <f t="shared" si="3"/>
         <v>43827</v>
@@ -1396,7 +1459,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A92" s="1">
         <f t="shared" si="3"/>
         <v>43828</v>
@@ -1406,7 +1469,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="93" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A93" s="1">
         <f t="shared" si="3"/>
         <v>43829</v>
@@ -1416,7 +1479,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="94" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A94" s="1">
         <f t="shared" si="3"/>
         <v>43830</v>
@@ -1426,13 +1489,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="95" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A95" s="1"/>
     </row>
-    <row r="96" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A96" s="1"/>
     </row>
-    <row r="97" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A97" s="1"/>
     </row>
   </sheetData>
@@ -1442,26 +1505,26 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:J97"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="18.6640625" defaultRowHeight="34.200000000000003" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="18.7109375" defaultRowHeight="34.15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.5546875" style="2" customWidth="1"/>
+    <col min="1" max="1" width="12.5703125" style="2" customWidth="1"/>
     <col min="2" max="2" width="19" style="2" customWidth="1"/>
-    <col min="3" max="16384" width="18.6640625" style="2"/>
+    <col min="3" max="16384" width="18.7109375" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B1" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -1493,7 +1556,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>43739</v>
       </c>
@@ -1507,7 +1570,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <f>A3+1</f>
         <v>43740</v>
@@ -1522,553 +1585,553 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <f t="shared" ref="A5:A68" si="0">A4+1</f>
         <v>43741</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
         <f t="shared" si="0"/>
         <v>43742</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
         <f t="shared" si="0"/>
         <v>43743</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
         <f t="shared" si="0"/>
         <v>43744</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
         <f t="shared" si="0"/>
         <v>43745</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
         <f t="shared" si="0"/>
         <v>43746</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
         <f t="shared" si="0"/>
         <v>43747</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="3">
         <f t="shared" si="0"/>
         <v>43748</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="3">
         <f t="shared" si="0"/>
         <v>43749</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:10" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="3">
         <f t="shared" si="0"/>
         <v>43750</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:10" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="3">
         <f t="shared" si="0"/>
         <v>43751</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:10" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="3">
         <f t="shared" si="0"/>
         <v>43752</v>
       </c>
     </row>
-    <row r="17" spans="1:1" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:1" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="3">
         <f t="shared" si="0"/>
         <v>43753</v>
       </c>
     </row>
-    <row r="18" spans="1:1" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:1" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="3">
         <f t="shared" si="0"/>
         <v>43754</v>
       </c>
     </row>
-    <row r="19" spans="1:1" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:1" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="3">
         <f t="shared" si="0"/>
         <v>43755</v>
       </c>
     </row>
-    <row r="20" spans="1:1" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:1" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="3">
         <f t="shared" si="0"/>
         <v>43756</v>
       </c>
     </row>
-    <row r="21" spans="1:1" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:1" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="3">
         <f t="shared" si="0"/>
         <v>43757</v>
       </c>
     </row>
-    <row r="22" spans="1:1" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:1" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="3">
         <f t="shared" si="0"/>
         <v>43758</v>
       </c>
     </row>
-    <row r="23" spans="1:1" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:1" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="3">
         <f t="shared" si="0"/>
         <v>43759</v>
       </c>
     </row>
-    <row r="24" spans="1:1" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:1" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="3">
         <f t="shared" si="0"/>
         <v>43760</v>
       </c>
     </row>
-    <row r="25" spans="1:1" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:1" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="3">
         <f t="shared" si="0"/>
         <v>43761</v>
       </c>
     </row>
-    <row r="26" spans="1:1" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:1" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="3">
         <f t="shared" si="0"/>
         <v>43762</v>
       </c>
     </row>
-    <row r="27" spans="1:1" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:1" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="3">
         <f t="shared" si="0"/>
         <v>43763</v>
       </c>
     </row>
-    <row r="28" spans="1:1" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:1" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="3">
         <f t="shared" si="0"/>
         <v>43764</v>
       </c>
     </row>
-    <row r="29" spans="1:1" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:1" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="3">
         <f t="shared" si="0"/>
         <v>43765</v>
       </c>
     </row>
-    <row r="30" spans="1:1" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:1" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="3">
         <f t="shared" si="0"/>
         <v>43766</v>
       </c>
     </row>
-    <row r="31" spans="1:1" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:1" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="3">
         <f t="shared" si="0"/>
         <v>43767</v>
       </c>
     </row>
-    <row r="32" spans="1:1" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:1" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="3">
         <f t="shared" si="0"/>
         <v>43768</v>
       </c>
     </row>
-    <row r="33" spans="1:1" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:1" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="3">
         <f t="shared" si="0"/>
         <v>43769</v>
       </c>
     </row>
-    <row r="34" spans="1:1" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:1" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="3">
         <f t="shared" si="0"/>
         <v>43770</v>
       </c>
     </row>
-    <row r="35" spans="1:1" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:1" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="3">
         <f t="shared" si="0"/>
         <v>43771</v>
       </c>
     </row>
-    <row r="36" spans="1:1" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:1" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="3">
         <f t="shared" si="0"/>
         <v>43772</v>
       </c>
     </row>
-    <row r="37" spans="1:1" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:1" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="3">
         <f t="shared" si="0"/>
         <v>43773</v>
       </c>
     </row>
-    <row r="38" spans="1:1" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:1" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="3">
         <f t="shared" si="0"/>
         <v>43774</v>
       </c>
     </row>
-    <row r="39" spans="1:1" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:1" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="3">
         <f t="shared" si="0"/>
         <v>43775</v>
       </c>
     </row>
-    <row r="40" spans="1:1" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:1" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="3">
         <f t="shared" si="0"/>
         <v>43776</v>
       </c>
     </row>
-    <row r="41" spans="1:1" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:1" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="3">
         <f t="shared" si="0"/>
         <v>43777</v>
       </c>
     </row>
-    <row r="42" spans="1:1" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:1" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="3">
         <f t="shared" si="0"/>
         <v>43778</v>
       </c>
     </row>
-    <row r="43" spans="1:1" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:1" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="3">
         <f t="shared" si="0"/>
         <v>43779</v>
       </c>
     </row>
-    <row r="44" spans="1:1" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:1" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="3">
         <f t="shared" si="0"/>
         <v>43780</v>
       </c>
     </row>
-    <row r="45" spans="1:1" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:1" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="3">
         <f t="shared" si="0"/>
         <v>43781</v>
       </c>
     </row>
-    <row r="46" spans="1:1" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:1" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="3">
         <f t="shared" si="0"/>
         <v>43782</v>
       </c>
     </row>
-    <row r="47" spans="1:1" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:1" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="3">
         <f t="shared" si="0"/>
         <v>43783</v>
       </c>
     </row>
-    <row r="48" spans="1:1" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:1" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="3">
         <f t="shared" si="0"/>
         <v>43784</v>
       </c>
     </row>
-    <row r="49" spans="1:1" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:1" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="3">
         <f t="shared" si="0"/>
         <v>43785</v>
       </c>
     </row>
-    <row r="50" spans="1:1" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:1" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="3">
         <f t="shared" si="0"/>
         <v>43786</v>
       </c>
     </row>
-    <row r="51" spans="1:1" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:1" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="3">
         <f t="shared" si="0"/>
         <v>43787</v>
       </c>
     </row>
-    <row r="52" spans="1:1" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:1" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="3">
         <f t="shared" si="0"/>
         <v>43788</v>
       </c>
     </row>
-    <row r="53" spans="1:1" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:1" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="3">
         <f t="shared" si="0"/>
         <v>43789</v>
       </c>
     </row>
-    <row r="54" spans="1:1" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:1" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="3">
         <f t="shared" si="0"/>
         <v>43790</v>
       </c>
     </row>
-    <row r="55" spans="1:1" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:1" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="3">
         <f t="shared" si="0"/>
         <v>43791</v>
       </c>
     </row>
-    <row r="56" spans="1:1" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:1" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="3">
         <f t="shared" si="0"/>
         <v>43792</v>
       </c>
     </row>
-    <row r="57" spans="1:1" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:1" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="3">
         <f t="shared" si="0"/>
         <v>43793</v>
       </c>
     </row>
-    <row r="58" spans="1:1" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:1" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="3">
         <f t="shared" si="0"/>
         <v>43794</v>
       </c>
     </row>
-    <row r="59" spans="1:1" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:1" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="3">
         <f t="shared" si="0"/>
         <v>43795</v>
       </c>
     </row>
-    <row r="60" spans="1:1" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:1" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="3">
         <f t="shared" si="0"/>
         <v>43796</v>
       </c>
     </row>
-    <row r="61" spans="1:1" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:1" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="3">
         <f t="shared" si="0"/>
         <v>43797</v>
       </c>
     </row>
-    <row r="62" spans="1:1" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:1" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="3">
         <f t="shared" si="0"/>
         <v>43798</v>
       </c>
     </row>
-    <row r="63" spans="1:1" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:1" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="3">
         <f t="shared" si="0"/>
         <v>43799</v>
       </c>
     </row>
-    <row r="64" spans="1:1" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:1" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="3">
         <f t="shared" si="0"/>
         <v>43800</v>
       </c>
     </row>
-    <row r="65" spans="1:1" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:1" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="3">
         <f t="shared" si="0"/>
         <v>43801</v>
       </c>
     </row>
-    <row r="66" spans="1:1" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:1" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" s="3">
         <f t="shared" si="0"/>
         <v>43802</v>
       </c>
     </row>
-    <row r="67" spans="1:1" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:1" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" s="3">
         <f t="shared" si="0"/>
         <v>43803</v>
       </c>
     </row>
-    <row r="68" spans="1:1" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:1" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="3">
         <f t="shared" si="0"/>
         <v>43804</v>
       </c>
     </row>
-    <row r="69" spans="1:1" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:1" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" s="3">
         <f t="shared" ref="A69:A94" si="1">A68+1</f>
         <v>43805</v>
       </c>
     </row>
-    <row r="70" spans="1:1" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:1" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" s="3">
         <f t="shared" si="1"/>
         <v>43806</v>
       </c>
     </row>
-    <row r="71" spans="1:1" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:1" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" s="3">
         <f t="shared" si="1"/>
         <v>43807</v>
       </c>
     </row>
-    <row r="72" spans="1:1" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:1" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" s="3">
         <f t="shared" si="1"/>
         <v>43808</v>
       </c>
     </row>
-    <row r="73" spans="1:1" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:1" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" s="3">
         <f t="shared" si="1"/>
         <v>43809</v>
       </c>
     </row>
-    <row r="74" spans="1:1" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:1" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" s="3">
         <f t="shared" si="1"/>
         <v>43810</v>
       </c>
     </row>
-    <row r="75" spans="1:1" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:1" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" s="3">
         <f t="shared" si="1"/>
         <v>43811</v>
       </c>
     </row>
-    <row r="76" spans="1:1" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:1" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76" s="3">
         <f t="shared" si="1"/>
         <v>43812</v>
       </c>
     </row>
-    <row r="77" spans="1:1" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:1" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A77" s="3">
         <f t="shared" si="1"/>
         <v>43813</v>
       </c>
     </row>
-    <row r="78" spans="1:1" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:1" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A78" s="3">
         <f t="shared" si="1"/>
         <v>43814</v>
       </c>
     </row>
-    <row r="79" spans="1:1" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:1" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A79" s="3">
         <f t="shared" si="1"/>
         <v>43815</v>
       </c>
     </row>
-    <row r="80" spans="1:1" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:1" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A80" s="3">
         <f t="shared" si="1"/>
         <v>43816</v>
       </c>
     </row>
-    <row r="81" spans="1:1" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:1" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A81" s="3">
         <f t="shared" si="1"/>
         <v>43817</v>
       </c>
     </row>
-    <row r="82" spans="1:1" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:1" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A82" s="3">
         <f t="shared" si="1"/>
         <v>43818</v>
       </c>
     </row>
-    <row r="83" spans="1:1" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:1" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A83" s="3">
         <f t="shared" si="1"/>
         <v>43819</v>
       </c>
     </row>
-    <row r="84" spans="1:1" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:1" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A84" s="3">
         <f t="shared" si="1"/>
         <v>43820</v>
       </c>
     </row>
-    <row r="85" spans="1:1" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:1" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A85" s="3">
         <f t="shared" si="1"/>
         <v>43821</v>
       </c>
     </row>
-    <row r="86" spans="1:1" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:1" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A86" s="3">
         <f t="shared" si="1"/>
         <v>43822</v>
       </c>
     </row>
-    <row r="87" spans="1:1" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:1" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A87" s="3">
         <f t="shared" si="1"/>
         <v>43823</v>
       </c>
     </row>
-    <row r="88" spans="1:1" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:1" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A88" s="3">
         <f t="shared" si="1"/>
         <v>43824</v>
       </c>
     </row>
-    <row r="89" spans="1:1" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:1" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A89" s="3">
         <f t="shared" si="1"/>
         <v>43825</v>
       </c>
     </row>
-    <row r="90" spans="1:1" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:1" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A90" s="3">
         <f t="shared" si="1"/>
         <v>43826</v>
       </c>
     </row>
-    <row r="91" spans="1:1" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:1" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A91" s="3">
         <f t="shared" si="1"/>
         <v>43827</v>
       </c>
     </row>
-    <row r="92" spans="1:1" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:1" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A92" s="3">
         <f t="shared" si="1"/>
         <v>43828</v>
       </c>
     </row>
-    <row r="93" spans="1:1" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:1" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A93" s="3">
         <f t="shared" si="1"/>
         <v>43829</v>
       </c>
     </row>
-    <row r="94" spans="1:1" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:1" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A94" s="3">
         <f t="shared" si="1"/>
         <v>43830</v>
       </c>
     </row>
-    <row r="95" spans="1:1" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:1" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A95" s="3"/>
     </row>
-    <row r="96" spans="1:1" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:1" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A96" s="3"/>
     </row>
-    <row r="97" spans="1:1" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:1" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A97" s="3"/>
     </row>
   </sheetData>
@@ -2077,12 +2140,12 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Update for 5th Oct
</commit_message>
<xml_diff>
--- a/ProgressExcel.xlsx
+++ b/ProgressExcel.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Anil\Courses\progressXL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3042E85-20BA-4861-8123-1CFED0E49645}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{327B565E-9EF5-4878-8036-F40A355AA9B4}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="16663" windowHeight="9017" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -478,31 +478,31 @@
   <dimension ref="A1:N97"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.69140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.3046875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.53515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.3046875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="4.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.3046875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.3828125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.15234375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.3828125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.3828125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.3046875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="4.84375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.4">
       <c r="B1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -537,7 +537,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A3" s="1">
         <v>43739</v>
       </c>
@@ -555,7 +555,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A4" s="1">
         <f>A3+1</f>
         <v>43740</v>
@@ -574,7 +574,7 @@
         <v>3.5</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A5" s="1">
         <f t="shared" ref="A5:A68" si="1">A4+1</f>
         <v>43741</v>
@@ -599,27 +599,48 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A6" s="1">
         <f t="shared" si="1"/>
         <v>43742</v>
       </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
       <c r="N6">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A7" s="1">
         <f t="shared" si="1"/>
         <v>43743</v>
       </c>
+      <c r="C7">
+        <v>5</v>
+      </c>
       <c r="N7">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A8" s="1">
         <f t="shared" si="1"/>
         <v>43744</v>
@@ -629,7 +650,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A9" s="1">
         <f t="shared" si="1"/>
         <v>43745</v>
@@ -639,7 +660,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A10" s="1">
         <f t="shared" si="1"/>
         <v>43746</v>
@@ -649,7 +670,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A11" s="1">
         <f t="shared" si="1"/>
         <v>43747</v>
@@ -659,7 +680,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A12" s="1">
         <f t="shared" si="1"/>
         <v>43748</v>
@@ -669,7 +690,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A13" s="1">
         <f t="shared" si="1"/>
         <v>43749</v>
@@ -679,7 +700,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A14" s="1">
         <f t="shared" si="1"/>
         <v>43750</v>
@@ -689,7 +710,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A15" s="1">
         <f t="shared" si="1"/>
         <v>43751</v>
@@ -699,7 +720,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A16" s="1">
         <f t="shared" si="1"/>
         <v>43752</v>
@@ -709,7 +730,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A17" s="1">
         <f t="shared" si="1"/>
         <v>43753</v>
@@ -719,7 +740,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A18" s="1">
         <f t="shared" si="1"/>
         <v>43754</v>
@@ -729,7 +750,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A19" s="1">
         <f t="shared" si="1"/>
         <v>43755</v>
@@ -739,7 +760,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A20" s="1">
         <f t="shared" si="1"/>
         <v>43756</v>
@@ -749,7 +770,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A21" s="1">
         <f t="shared" si="1"/>
         <v>43757</v>
@@ -759,7 +780,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A22" s="1">
         <f t="shared" si="1"/>
         <v>43758</v>
@@ -769,7 +790,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A23" s="1">
         <f t="shared" si="1"/>
         <v>43759</v>
@@ -779,7 +800,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A24" s="1">
         <f t="shared" si="1"/>
         <v>43760</v>
@@ -789,7 +810,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A25" s="1">
         <f t="shared" si="1"/>
         <v>43761</v>
@@ -799,7 +820,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A26" s="1">
         <f t="shared" si="1"/>
         <v>43762</v>
@@ -809,7 +830,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A27" s="1">
         <f t="shared" si="1"/>
         <v>43763</v>
@@ -819,7 +840,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A28" s="1">
         <f t="shared" si="1"/>
         <v>43764</v>
@@ -829,7 +850,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A29" s="1">
         <f t="shared" si="1"/>
         <v>43765</v>
@@ -839,7 +860,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A30" s="1">
         <f t="shared" si="1"/>
         <v>43766</v>
@@ -849,7 +870,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A31" s="1">
         <f t="shared" si="1"/>
         <v>43767</v>
@@ -859,7 +880,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A32" s="1">
         <f t="shared" si="1"/>
         <v>43768</v>
@@ -869,7 +890,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A33" s="1">
         <f t="shared" si="1"/>
         <v>43769</v>
@@ -879,7 +900,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A34" s="1">
         <f t="shared" si="1"/>
         <v>43770</v>
@@ -889,7 +910,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A35" s="1">
         <f t="shared" si="1"/>
         <v>43771</v>
@@ -899,7 +920,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A36" s="1">
         <f t="shared" si="1"/>
         <v>43772</v>
@@ -909,7 +930,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A37" s="1">
         <f t="shared" si="1"/>
         <v>43773</v>
@@ -919,7 +940,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A38" s="1">
         <f t="shared" si="1"/>
         <v>43774</v>
@@ -929,7 +950,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A39" s="1">
         <f t="shared" si="1"/>
         <v>43775</v>
@@ -939,7 +960,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A40" s="1">
         <f t="shared" si="1"/>
         <v>43776</v>
@@ -949,7 +970,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A41" s="1">
         <f t="shared" si="1"/>
         <v>43777</v>
@@ -959,7 +980,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A42" s="1">
         <f t="shared" si="1"/>
         <v>43778</v>
@@ -969,7 +990,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A43" s="1">
         <f t="shared" si="1"/>
         <v>43779</v>
@@ -979,7 +1000,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A44" s="1">
         <f t="shared" si="1"/>
         <v>43780</v>
@@ -989,7 +1010,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A45" s="1">
         <f t="shared" si="1"/>
         <v>43781</v>
@@ -999,7 +1020,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A46" s="1">
         <f t="shared" si="1"/>
         <v>43782</v>
@@ -1009,7 +1030,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A47" s="1">
         <f t="shared" si="1"/>
         <v>43783</v>
@@ -1019,7 +1040,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A48" s="1">
         <f t="shared" si="1"/>
         <v>43784</v>
@@ -1029,7 +1050,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A49" s="1">
         <f t="shared" si="1"/>
         <v>43785</v>
@@ -1039,7 +1060,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A50" s="1">
         <f t="shared" si="1"/>
         <v>43786</v>
@@ -1049,7 +1070,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A51" s="1">
         <f t="shared" si="1"/>
         <v>43787</v>
@@ -1059,7 +1080,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A52" s="1">
         <f t="shared" si="1"/>
         <v>43788</v>
@@ -1069,7 +1090,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A53" s="1">
         <f t="shared" si="1"/>
         <v>43789</v>
@@ -1079,7 +1100,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A54" s="1">
         <f t="shared" si="1"/>
         <v>43790</v>
@@ -1089,7 +1110,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A55" s="1">
         <f t="shared" si="1"/>
         <v>43791</v>
@@ -1099,7 +1120,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A56" s="1">
         <f t="shared" si="1"/>
         <v>43792</v>
@@ -1109,7 +1130,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A57" s="1">
         <f t="shared" si="1"/>
         <v>43793</v>
@@ -1119,7 +1140,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A58" s="1">
         <f t="shared" si="1"/>
         <v>43794</v>
@@ -1129,7 +1150,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A59" s="1">
         <f t="shared" si="1"/>
         <v>43795</v>
@@ -1139,7 +1160,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A60" s="1">
         <f t="shared" si="1"/>
         <v>43796</v>
@@ -1149,7 +1170,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A61" s="1">
         <f t="shared" si="1"/>
         <v>43797</v>
@@ -1159,7 +1180,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A62" s="1">
         <f t="shared" si="1"/>
         <v>43798</v>
@@ -1169,7 +1190,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A63" s="1">
         <f t="shared" si="1"/>
         <v>43799</v>
@@ -1179,7 +1200,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A64" s="1">
         <f t="shared" si="1"/>
         <v>43800</v>
@@ -1189,7 +1210,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A65" s="1">
         <f t="shared" si="1"/>
         <v>43801</v>
@@ -1199,7 +1220,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A66" s="1">
         <f t="shared" si="1"/>
         <v>43802</v>
@@ -1209,7 +1230,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A67" s="1">
         <f t="shared" si="1"/>
         <v>43803</v>
@@ -1219,7 +1240,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A68" s="1">
         <f t="shared" si="1"/>
         <v>43804</v>
@@ -1229,7 +1250,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A69" s="1">
         <f t="shared" ref="A69:A94" si="3">A68+1</f>
         <v>43805</v>
@@ -1239,7 +1260,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A70" s="1">
         <f t="shared" si="3"/>
         <v>43806</v>
@@ -1249,7 +1270,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A71" s="1">
         <f t="shared" si="3"/>
         <v>43807</v>
@@ -1259,7 +1280,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A72" s="1">
         <f t="shared" si="3"/>
         <v>43808</v>
@@ -1269,7 +1290,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A73" s="1">
         <f t="shared" si="3"/>
         <v>43809</v>
@@ -1279,7 +1300,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A74" s="1">
         <f t="shared" si="3"/>
         <v>43810</v>
@@ -1289,7 +1310,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A75" s="1">
         <f t="shared" si="3"/>
         <v>43811</v>
@@ -1299,7 +1320,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A76" s="1">
         <f t="shared" si="3"/>
         <v>43812</v>
@@ -1309,7 +1330,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A77" s="1">
         <f t="shared" si="3"/>
         <v>43813</v>
@@ -1319,7 +1340,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A78" s="1">
         <f t="shared" si="3"/>
         <v>43814</v>
@@ -1329,7 +1350,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A79" s="1">
         <f t="shared" si="3"/>
         <v>43815</v>
@@ -1339,7 +1360,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A80" s="1">
         <f t="shared" si="3"/>
         <v>43816</v>
@@ -1349,7 +1370,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A81" s="1">
         <f t="shared" si="3"/>
         <v>43817</v>
@@ -1359,7 +1380,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A82" s="1">
         <f t="shared" si="3"/>
         <v>43818</v>
@@ -1369,7 +1390,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A83" s="1">
         <f t="shared" si="3"/>
         <v>43819</v>
@@ -1379,7 +1400,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A84" s="1">
         <f t="shared" si="3"/>
         <v>43820</v>
@@ -1389,7 +1410,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A85" s="1">
         <f t="shared" si="3"/>
         <v>43821</v>
@@ -1399,7 +1420,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A86" s="1">
         <f t="shared" si="3"/>
         <v>43822</v>
@@ -1409,7 +1430,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A87" s="1">
         <f t="shared" si="3"/>
         <v>43823</v>
@@ -1419,7 +1440,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A88" s="1">
         <f t="shared" si="3"/>
         <v>43824</v>
@@ -1429,7 +1450,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A89" s="1">
         <f t="shared" si="3"/>
         <v>43825</v>
@@ -1439,7 +1460,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A90" s="1">
         <f t="shared" si="3"/>
         <v>43826</v>
@@ -1449,7 +1470,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="91" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A91" s="1">
         <f t="shared" si="3"/>
         <v>43827</v>
@@ -1459,7 +1480,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A92" s="1">
         <f t="shared" si="3"/>
         <v>43828</v>
@@ -1469,7 +1490,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="93" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A93" s="1">
         <f t="shared" si="3"/>
         <v>43829</v>
@@ -1479,7 +1500,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="94" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A94" s="1">
         <f t="shared" si="3"/>
         <v>43830</v>
@@ -1489,13 +1510,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="95" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A95" s="1"/>
     </row>
-    <row r="96" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A96" s="1"/>
     </row>
-    <row r="97" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A97" s="1"/>
     </row>
   </sheetData>
@@ -1512,19 +1533,19 @@
       <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="18.7109375" defaultRowHeight="34.15" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="18.69140625" defaultRowHeight="34.200000000000003" customHeight="1" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="12.5703125" style="2" customWidth="1"/>
+    <col min="1" max="1" width="12.53515625" style="2" customWidth="1"/>
     <col min="2" max="2" width="19" style="2" customWidth="1"/>
-    <col min="3" max="16384" width="18.7109375" style="2"/>
+    <col min="3" max="16384" width="18.69140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B1" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -1556,7 +1577,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A3" s="3">
         <v>43739</v>
       </c>
@@ -1570,7 +1591,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A4" s="3">
         <f>A3+1</f>
         <v>43740</v>
@@ -1585,553 +1606,553 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A5" s="3">
         <f t="shared" ref="A5:A68" si="0">A4+1</f>
         <v>43741</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A6" s="3">
         <f t="shared" si="0"/>
         <v>43742</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A7" s="3">
         <f t="shared" si="0"/>
         <v>43743</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A8" s="3">
         <f t="shared" si="0"/>
         <v>43744</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A9" s="3">
         <f t="shared" si="0"/>
         <v>43745</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A10" s="3">
         <f t="shared" si="0"/>
         <v>43746</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A11" s="3">
         <f t="shared" si="0"/>
         <v>43747</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A12" s="3">
         <f t="shared" si="0"/>
         <v>43748</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A13" s="3">
         <f t="shared" si="0"/>
         <v>43749</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A14" s="3">
         <f t="shared" si="0"/>
         <v>43750</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A15" s="3">
         <f t="shared" si="0"/>
         <v>43751</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A16" s="3">
         <f t="shared" si="0"/>
         <v>43752</v>
       </c>
     </row>
-    <row r="17" spans="1:1" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:1" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A17" s="3">
         <f t="shared" si="0"/>
         <v>43753</v>
       </c>
     </row>
-    <row r="18" spans="1:1" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:1" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A18" s="3">
         <f t="shared" si="0"/>
         <v>43754</v>
       </c>
     </row>
-    <row r="19" spans="1:1" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:1" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A19" s="3">
         <f t="shared" si="0"/>
         <v>43755</v>
       </c>
     </row>
-    <row r="20" spans="1:1" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:1" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A20" s="3">
         <f t="shared" si="0"/>
         <v>43756</v>
       </c>
     </row>
-    <row r="21" spans="1:1" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:1" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A21" s="3">
         <f t="shared" si="0"/>
         <v>43757</v>
       </c>
     </row>
-    <row r="22" spans="1:1" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:1" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A22" s="3">
         <f t="shared" si="0"/>
         <v>43758</v>
       </c>
     </row>
-    <row r="23" spans="1:1" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:1" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A23" s="3">
         <f t="shared" si="0"/>
         <v>43759</v>
       </c>
     </row>
-    <row r="24" spans="1:1" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:1" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A24" s="3">
         <f t="shared" si="0"/>
         <v>43760</v>
       </c>
     </row>
-    <row r="25" spans="1:1" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:1" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A25" s="3">
         <f t="shared" si="0"/>
         <v>43761</v>
       </c>
     </row>
-    <row r="26" spans="1:1" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:1" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A26" s="3">
         <f t="shared" si="0"/>
         <v>43762</v>
       </c>
     </row>
-    <row r="27" spans="1:1" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:1" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A27" s="3">
         <f t="shared" si="0"/>
         <v>43763</v>
       </c>
     </row>
-    <row r="28" spans="1:1" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:1" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A28" s="3">
         <f t="shared" si="0"/>
         <v>43764</v>
       </c>
     </row>
-    <row r="29" spans="1:1" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:1" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A29" s="3">
         <f t="shared" si="0"/>
         <v>43765</v>
       </c>
     </row>
-    <row r="30" spans="1:1" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:1" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A30" s="3">
         <f t="shared" si="0"/>
         <v>43766</v>
       </c>
     </row>
-    <row r="31" spans="1:1" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:1" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A31" s="3">
         <f t="shared" si="0"/>
         <v>43767</v>
       </c>
     </row>
-    <row r="32" spans="1:1" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:1" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A32" s="3">
         <f t="shared" si="0"/>
         <v>43768</v>
       </c>
     </row>
-    <row r="33" spans="1:1" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:1" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A33" s="3">
         <f t="shared" si="0"/>
         <v>43769</v>
       </c>
     </row>
-    <row r="34" spans="1:1" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:1" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A34" s="3">
         <f t="shared" si="0"/>
         <v>43770</v>
       </c>
     </row>
-    <row r="35" spans="1:1" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:1" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A35" s="3">
         <f t="shared" si="0"/>
         <v>43771</v>
       </c>
     </row>
-    <row r="36" spans="1:1" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:1" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A36" s="3">
         <f t="shared" si="0"/>
         <v>43772</v>
       </c>
     </row>
-    <row r="37" spans="1:1" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:1" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A37" s="3">
         <f t="shared" si="0"/>
         <v>43773</v>
       </c>
     </row>
-    <row r="38" spans="1:1" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:1" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A38" s="3">
         <f t="shared" si="0"/>
         <v>43774</v>
       </c>
     </row>
-    <row r="39" spans="1:1" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:1" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A39" s="3">
         <f t="shared" si="0"/>
         <v>43775</v>
       </c>
     </row>
-    <row r="40" spans="1:1" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:1" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A40" s="3">
         <f t="shared" si="0"/>
         <v>43776</v>
       </c>
     </row>
-    <row r="41" spans="1:1" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:1" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A41" s="3">
         <f t="shared" si="0"/>
         <v>43777</v>
       </c>
     </row>
-    <row r="42" spans="1:1" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:1" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A42" s="3">
         <f t="shared" si="0"/>
         <v>43778</v>
       </c>
     </row>
-    <row r="43" spans="1:1" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:1" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A43" s="3">
         <f t="shared" si="0"/>
         <v>43779</v>
       </c>
     </row>
-    <row r="44" spans="1:1" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:1" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A44" s="3">
         <f t="shared" si="0"/>
         <v>43780</v>
       </c>
     </row>
-    <row r="45" spans="1:1" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:1" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A45" s="3">
         <f t="shared" si="0"/>
         <v>43781</v>
       </c>
     </row>
-    <row r="46" spans="1:1" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:1" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A46" s="3">
         <f t="shared" si="0"/>
         <v>43782</v>
       </c>
     </row>
-    <row r="47" spans="1:1" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:1" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A47" s="3">
         <f t="shared" si="0"/>
         <v>43783</v>
       </c>
     </row>
-    <row r="48" spans="1:1" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:1" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A48" s="3">
         <f t="shared" si="0"/>
         <v>43784</v>
       </c>
     </row>
-    <row r="49" spans="1:1" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:1" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A49" s="3">
         <f t="shared" si="0"/>
         <v>43785</v>
       </c>
     </row>
-    <row r="50" spans="1:1" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:1" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A50" s="3">
         <f t="shared" si="0"/>
         <v>43786</v>
       </c>
     </row>
-    <row r="51" spans="1:1" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:1" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A51" s="3">
         <f t="shared" si="0"/>
         <v>43787</v>
       </c>
     </row>
-    <row r="52" spans="1:1" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:1" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A52" s="3">
         <f t="shared" si="0"/>
         <v>43788</v>
       </c>
     </row>
-    <row r="53" spans="1:1" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:1" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A53" s="3">
         <f t="shared" si="0"/>
         <v>43789</v>
       </c>
     </row>
-    <row r="54" spans="1:1" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:1" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A54" s="3">
         <f t="shared" si="0"/>
         <v>43790</v>
       </c>
     </row>
-    <row r="55" spans="1:1" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:1" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A55" s="3">
         <f t="shared" si="0"/>
         <v>43791</v>
       </c>
     </row>
-    <row r="56" spans="1:1" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:1" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A56" s="3">
         <f t="shared" si="0"/>
         <v>43792</v>
       </c>
     </row>
-    <row r="57" spans="1:1" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:1" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A57" s="3">
         <f t="shared" si="0"/>
         <v>43793</v>
       </c>
     </row>
-    <row r="58" spans="1:1" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:1" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A58" s="3">
         <f t="shared" si="0"/>
         <v>43794</v>
       </c>
     </row>
-    <row r="59" spans="1:1" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:1" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A59" s="3">
         <f t="shared" si="0"/>
         <v>43795</v>
       </c>
     </row>
-    <row r="60" spans="1:1" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:1" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A60" s="3">
         <f t="shared" si="0"/>
         <v>43796</v>
       </c>
     </row>
-    <row r="61" spans="1:1" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:1" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A61" s="3">
         <f t="shared" si="0"/>
         <v>43797</v>
       </c>
     </row>
-    <row r="62" spans="1:1" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:1" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A62" s="3">
         <f t="shared" si="0"/>
         <v>43798</v>
       </c>
     </row>
-    <row r="63" spans="1:1" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:1" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A63" s="3">
         <f t="shared" si="0"/>
         <v>43799</v>
       </c>
     </row>
-    <row r="64" spans="1:1" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:1" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A64" s="3">
         <f t="shared" si="0"/>
         <v>43800</v>
       </c>
     </row>
-    <row r="65" spans="1:1" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:1" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A65" s="3">
         <f t="shared" si="0"/>
         <v>43801</v>
       </c>
     </row>
-    <row r="66" spans="1:1" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:1" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A66" s="3">
         <f t="shared" si="0"/>
         <v>43802</v>
       </c>
     </row>
-    <row r="67" spans="1:1" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:1" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A67" s="3">
         <f t="shared" si="0"/>
         <v>43803</v>
       </c>
     </row>
-    <row r="68" spans="1:1" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:1" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A68" s="3">
         <f t="shared" si="0"/>
         <v>43804</v>
       </c>
     </row>
-    <row r="69" spans="1:1" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:1" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A69" s="3">
         <f t="shared" ref="A69:A94" si="1">A68+1</f>
         <v>43805</v>
       </c>
     </row>
-    <row r="70" spans="1:1" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:1" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A70" s="3">
         <f t="shared" si="1"/>
         <v>43806</v>
       </c>
     </row>
-    <row r="71" spans="1:1" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:1" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A71" s="3">
         <f t="shared" si="1"/>
         <v>43807</v>
       </c>
     </row>
-    <row r="72" spans="1:1" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:1" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A72" s="3">
         <f t="shared" si="1"/>
         <v>43808</v>
       </c>
     </row>
-    <row r="73" spans="1:1" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:1" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A73" s="3">
         <f t="shared" si="1"/>
         <v>43809</v>
       </c>
     </row>
-    <row r="74" spans="1:1" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:1" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A74" s="3">
         <f t="shared" si="1"/>
         <v>43810</v>
       </c>
     </row>
-    <row r="75" spans="1:1" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:1" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A75" s="3">
         <f t="shared" si="1"/>
         <v>43811</v>
       </c>
     </row>
-    <row r="76" spans="1:1" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:1" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A76" s="3">
         <f t="shared" si="1"/>
         <v>43812</v>
       </c>
     </row>
-    <row r="77" spans="1:1" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:1" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A77" s="3">
         <f t="shared" si="1"/>
         <v>43813</v>
       </c>
     </row>
-    <row r="78" spans="1:1" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:1" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A78" s="3">
         <f t="shared" si="1"/>
         <v>43814</v>
       </c>
     </row>
-    <row r="79" spans="1:1" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:1" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A79" s="3">
         <f t="shared" si="1"/>
         <v>43815</v>
       </c>
     </row>
-    <row r="80" spans="1:1" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:1" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A80" s="3">
         <f t="shared" si="1"/>
         <v>43816</v>
       </c>
     </row>
-    <row r="81" spans="1:1" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:1" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A81" s="3">
         <f t="shared" si="1"/>
         <v>43817</v>
       </c>
     </row>
-    <row r="82" spans="1:1" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:1" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A82" s="3">
         <f t="shared" si="1"/>
         <v>43818</v>
       </c>
     </row>
-    <row r="83" spans="1:1" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:1" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A83" s="3">
         <f t="shared" si="1"/>
         <v>43819</v>
       </c>
     </row>
-    <row r="84" spans="1:1" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:1" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A84" s="3">
         <f t="shared" si="1"/>
         <v>43820</v>
       </c>
     </row>
-    <row r="85" spans="1:1" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:1" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A85" s="3">
         <f t="shared" si="1"/>
         <v>43821</v>
       </c>
     </row>
-    <row r="86" spans="1:1" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:1" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A86" s="3">
         <f t="shared" si="1"/>
         <v>43822</v>
       </c>
     </row>
-    <row r="87" spans="1:1" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:1" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A87" s="3">
         <f t="shared" si="1"/>
         <v>43823</v>
       </c>
     </row>
-    <row r="88" spans="1:1" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:1" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A88" s="3">
         <f t="shared" si="1"/>
         <v>43824</v>
       </c>
     </row>
-    <row r="89" spans="1:1" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:1" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A89" s="3">
         <f t="shared" si="1"/>
         <v>43825</v>
       </c>
     </row>
-    <row r="90" spans="1:1" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:1" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A90" s="3">
         <f t="shared" si="1"/>
         <v>43826</v>
       </c>
     </row>
-    <row r="91" spans="1:1" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:1" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A91" s="3">
         <f t="shared" si="1"/>
         <v>43827</v>
       </c>
     </row>
-    <row r="92" spans="1:1" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:1" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A92" s="3">
         <f t="shared" si="1"/>
         <v>43828</v>
       </c>
     </row>
-    <row r="93" spans="1:1" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:1" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A93" s="3">
         <f t="shared" si="1"/>
         <v>43829</v>
       </c>
     </row>
-    <row r="94" spans="1:1" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:1" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A94" s="3">
         <f t="shared" si="1"/>
         <v>43830</v>
       </c>
     </row>
-    <row r="95" spans="1:1" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:1" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A95" s="3"/>
     </row>
-    <row r="96" spans="1:1" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:1" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A96" s="3"/>
     </row>
-    <row r="97" spans="1:1" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:1" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A97" s="3"/>
     </row>
   </sheetData>
@@ -2145,7 +2166,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Update for 6th Oct and 7th Ovct
</commit_message>
<xml_diff>
--- a/ProgressExcel.xlsx
+++ b/ProgressExcel.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22026"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Anil\Courses\progressXL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{327B565E-9EF5-4878-8036-F40A355AA9B4}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E7FE906-0DB9-46EC-B76E-927908A4B0A5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-103" yWindow="-103" windowWidth="16663" windowHeight="9017" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -478,31 +478,31 @@
   <dimension ref="A1:N97"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="N5" sqref="N5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.69140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.3046875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.53515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.3046875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.3046875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.3828125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.15234375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.3828125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.3828125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.3046875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="4.84375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="4.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -537,7 +537,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>43739</v>
       </c>
@@ -555,7 +555,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <f>A3+1</f>
         <v>43740</v>
@@ -574,7 +574,7 @@
         <v>3.5</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <f t="shared" ref="A5:A68" si="1">A4+1</f>
         <v>43741</v>
@@ -595,11 +595,11 @@
         <v>0</v>
       </c>
       <c r="N5">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.4">
+        <f t="shared" ref="N5:N36" si="2">SUM(C5:K5)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <f t="shared" si="1"/>
         <v>43742</v>
@@ -623,11 +623,11 @@
         <v>0</v>
       </c>
       <c r="N6">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.4">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <f t="shared" si="1"/>
         <v>43743</v>
@@ -635,888 +635,924 @@
       <c r="C7">
         <v>5</v>
       </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
+      <c r="H7">
+        <v>0</v>
+      </c>
       <c r="N7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <f t="shared" si="1"/>
         <v>43744</v>
       </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+      <c r="F8">
+        <v>0</v>
+      </c>
+      <c r="G8">
+        <v>0</v>
+      </c>
+      <c r="H8">
+        <v>0</v>
+      </c>
       <c r="N8">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.4">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <f t="shared" si="1"/>
         <v>43745</v>
       </c>
+      <c r="K9">
+        <v>2</v>
+      </c>
       <c r="N9">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.4">
+        <f>SUM(C9:K9)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <f t="shared" si="1"/>
         <v>43746</v>
       </c>
       <c r="N10">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.4">
+        <f t="shared" ref="N10:N73" si="3">SUM(C10:K10)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <f t="shared" si="1"/>
         <v>43747</v>
       </c>
       <c r="N11">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.4">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <f t="shared" si="1"/>
         <v>43748</v>
       </c>
       <c r="N12">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.4">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <f t="shared" si="1"/>
         <v>43749</v>
       </c>
       <c r="N13">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.4">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <f t="shared" si="1"/>
         <v>43750</v>
       </c>
       <c r="N14">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.4">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <f t="shared" si="1"/>
         <v>43751</v>
       </c>
       <c r="N15">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.4">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <f t="shared" si="1"/>
         <v>43752</v>
       </c>
       <c r="N16">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.4">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <f t="shared" si="1"/>
         <v>43753</v>
       </c>
       <c r="N17">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.4">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <f t="shared" si="1"/>
         <v>43754</v>
       </c>
       <c r="N18">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.4">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <f t="shared" si="1"/>
         <v>43755</v>
       </c>
       <c r="N19">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.4">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <f t="shared" si="1"/>
         <v>43756</v>
       </c>
       <c r="N20">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.4">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <f t="shared" si="1"/>
         <v>43757</v>
       </c>
       <c r="N21">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.4">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <f t="shared" si="1"/>
         <v>43758</v>
       </c>
       <c r="N22">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.4">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <f t="shared" si="1"/>
         <v>43759</v>
       </c>
       <c r="N23">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.4">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <f t="shared" si="1"/>
         <v>43760</v>
       </c>
       <c r="N24">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.4">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <f t="shared" si="1"/>
         <v>43761</v>
       </c>
       <c r="N25">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.4">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <f t="shared" si="1"/>
         <v>43762</v>
       </c>
       <c r="N26">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.4">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <f t="shared" si="1"/>
         <v>43763</v>
       </c>
       <c r="N27">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.4">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <f t="shared" si="1"/>
         <v>43764</v>
       </c>
       <c r="N28">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.4">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <f t="shared" si="1"/>
         <v>43765</v>
       </c>
       <c r="N29">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.4">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <f t="shared" si="1"/>
         <v>43766</v>
       </c>
       <c r="N30">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.4">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <f t="shared" si="1"/>
         <v>43767</v>
       </c>
       <c r="N31">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.4">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <f t="shared" si="1"/>
         <v>43768</v>
       </c>
       <c r="N32">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.4">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <f t="shared" si="1"/>
         <v>43769</v>
       </c>
       <c r="N33">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.4">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <f t="shared" si="1"/>
         <v>43770</v>
       </c>
       <c r="N34">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.4">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <f t="shared" si="1"/>
         <v>43771</v>
       </c>
       <c r="N35">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.4">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <f t="shared" si="1"/>
         <v>43772</v>
       </c>
       <c r="N36">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.4">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <f t="shared" si="1"/>
         <v>43773</v>
       </c>
       <c r="N37">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.4">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <f t="shared" si="1"/>
         <v>43774</v>
       </c>
       <c r="N38">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.4">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <f t="shared" si="1"/>
         <v>43775</v>
       </c>
       <c r="N39">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="40" spans="1:14" x14ac:dyDescent="0.4">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <f t="shared" si="1"/>
         <v>43776</v>
       </c>
       <c r="N40">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="41" spans="1:14" x14ac:dyDescent="0.4">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <f t="shared" si="1"/>
         <v>43777</v>
       </c>
       <c r="N41">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="42" spans="1:14" x14ac:dyDescent="0.4">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
         <f t="shared" si="1"/>
         <v>43778</v>
       </c>
       <c r="N42">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="43" spans="1:14" x14ac:dyDescent="0.4">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
         <f t="shared" si="1"/>
         <v>43779</v>
       </c>
       <c r="N43">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="44" spans="1:14" x14ac:dyDescent="0.4">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
         <f t="shared" si="1"/>
         <v>43780</v>
       </c>
       <c r="N44">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="45" spans="1:14" x14ac:dyDescent="0.4">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
         <f t="shared" si="1"/>
         <v>43781</v>
       </c>
       <c r="N45">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="46" spans="1:14" x14ac:dyDescent="0.4">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
         <f t="shared" si="1"/>
         <v>43782</v>
       </c>
       <c r="N46">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="47" spans="1:14" x14ac:dyDescent="0.4">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
         <f t="shared" si="1"/>
         <v>43783</v>
       </c>
       <c r="N47">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="48" spans="1:14" x14ac:dyDescent="0.4">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
         <f t="shared" si="1"/>
         <v>43784</v>
       </c>
       <c r="N48">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="49" spans="1:14" x14ac:dyDescent="0.4">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
         <f t="shared" si="1"/>
         <v>43785</v>
       </c>
       <c r="N49">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="50" spans="1:14" x14ac:dyDescent="0.4">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
         <f t="shared" si="1"/>
         <v>43786</v>
       </c>
       <c r="N50">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="51" spans="1:14" x14ac:dyDescent="0.4">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
         <f t="shared" si="1"/>
         <v>43787</v>
       </c>
       <c r="N51">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="52" spans="1:14" x14ac:dyDescent="0.4">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A52" s="1">
         <f t="shared" si="1"/>
         <v>43788</v>
       </c>
       <c r="N52">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="53" spans="1:14" x14ac:dyDescent="0.4">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A53" s="1">
         <f t="shared" si="1"/>
         <v>43789</v>
       </c>
       <c r="N53">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="54" spans="1:14" x14ac:dyDescent="0.4">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A54" s="1">
         <f t="shared" si="1"/>
         <v>43790</v>
       </c>
       <c r="N54">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="55" spans="1:14" x14ac:dyDescent="0.4">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A55" s="1">
         <f t="shared" si="1"/>
         <v>43791</v>
       </c>
       <c r="N55">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="56" spans="1:14" x14ac:dyDescent="0.4">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A56" s="1">
         <f t="shared" si="1"/>
         <v>43792</v>
       </c>
       <c r="N56">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="57" spans="1:14" x14ac:dyDescent="0.4">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A57" s="1">
         <f t="shared" si="1"/>
         <v>43793</v>
       </c>
       <c r="N57">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="58" spans="1:14" x14ac:dyDescent="0.4">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A58" s="1">
         <f t="shared" si="1"/>
         <v>43794</v>
       </c>
       <c r="N58">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="59" spans="1:14" x14ac:dyDescent="0.4">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A59" s="1">
         <f t="shared" si="1"/>
         <v>43795</v>
       </c>
       <c r="N59">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="60" spans="1:14" x14ac:dyDescent="0.4">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A60" s="1">
         <f t="shared" si="1"/>
         <v>43796</v>
       </c>
       <c r="N60">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="61" spans="1:14" x14ac:dyDescent="0.4">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A61" s="1">
         <f t="shared" si="1"/>
         <v>43797</v>
       </c>
       <c r="N61">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="62" spans="1:14" x14ac:dyDescent="0.4">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A62" s="1">
         <f t="shared" si="1"/>
         <v>43798</v>
       </c>
       <c r="N62">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="63" spans="1:14" x14ac:dyDescent="0.4">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A63" s="1">
         <f t="shared" si="1"/>
         <v>43799</v>
       </c>
       <c r="N63">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="64" spans="1:14" x14ac:dyDescent="0.4">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A64" s="1">
         <f t="shared" si="1"/>
         <v>43800</v>
       </c>
       <c r="N64">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="65" spans="1:14" x14ac:dyDescent="0.4">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A65" s="1">
         <f t="shared" si="1"/>
         <v>43801</v>
       </c>
       <c r="N65">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="66" spans="1:14" x14ac:dyDescent="0.4">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A66" s="1">
         <f t="shared" si="1"/>
         <v>43802</v>
       </c>
       <c r="N66">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="67" spans="1:14" x14ac:dyDescent="0.4">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A67" s="1">
         <f t="shared" si="1"/>
         <v>43803</v>
       </c>
       <c r="N67">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="68" spans="1:14" x14ac:dyDescent="0.4">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A68" s="1">
         <f t="shared" si="1"/>
         <v>43804</v>
       </c>
       <c r="N68">
-        <f t="shared" ref="N68:N94" si="2">SUM(C68:J68)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="69" spans="1:14" x14ac:dyDescent="0.4">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A69" s="1">
-        <f t="shared" ref="A69:A94" si="3">A68+1</f>
+        <f t="shared" ref="A69:A94" si="4">A68+1</f>
         <v>43805</v>
       </c>
       <c r="N69">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="70" spans="1:14" x14ac:dyDescent="0.4">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A70" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>43806</v>
       </c>
       <c r="N70">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="71" spans="1:14" x14ac:dyDescent="0.4">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A71" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>43807</v>
       </c>
       <c r="N71">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="72" spans="1:14" x14ac:dyDescent="0.4">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A72" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>43808</v>
       </c>
       <c r="N72">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="73" spans="1:14" x14ac:dyDescent="0.4">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A73" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>43809</v>
       </c>
       <c r="N73">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="74" spans="1:14" x14ac:dyDescent="0.4">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A74" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>43810</v>
       </c>
       <c r="N74">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="75" spans="1:14" x14ac:dyDescent="0.4">
+        <f t="shared" ref="N74:N94" si="5">SUM(C74:K74)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A75" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>43811</v>
       </c>
       <c r="N75">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="76" spans="1:14" x14ac:dyDescent="0.4">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A76" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>43812</v>
       </c>
       <c r="N76">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="77" spans="1:14" x14ac:dyDescent="0.4">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A77" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>43813</v>
       </c>
       <c r="N77">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="78" spans="1:14" x14ac:dyDescent="0.4">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A78" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>43814</v>
       </c>
       <c r="N78">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="79" spans="1:14" x14ac:dyDescent="0.4">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A79" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>43815</v>
       </c>
       <c r="N79">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="80" spans="1:14" x14ac:dyDescent="0.4">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A80" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>43816</v>
       </c>
       <c r="N80">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="81" spans="1:14" x14ac:dyDescent="0.4">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A81" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>43817</v>
       </c>
       <c r="N81">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="82" spans="1:14" x14ac:dyDescent="0.4">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A82" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>43818</v>
       </c>
       <c r="N82">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="83" spans="1:14" x14ac:dyDescent="0.4">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A83" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>43819</v>
       </c>
       <c r="N83">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="84" spans="1:14" x14ac:dyDescent="0.4">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A84" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>43820</v>
       </c>
       <c r="N84">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="85" spans="1:14" x14ac:dyDescent="0.4">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A85" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>43821</v>
       </c>
       <c r="N85">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="86" spans="1:14" x14ac:dyDescent="0.4">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A86" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>43822</v>
       </c>
       <c r="N86">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="87" spans="1:14" x14ac:dyDescent="0.4">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A87" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>43823</v>
       </c>
       <c r="N87">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="88" spans="1:14" x14ac:dyDescent="0.4">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A88" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>43824</v>
       </c>
       <c r="N88">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="89" spans="1:14" x14ac:dyDescent="0.4">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A89" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>43825</v>
       </c>
       <c r="N89">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="90" spans="1:14" x14ac:dyDescent="0.4">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A90" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>43826</v>
       </c>
       <c r="N90">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="91" spans="1:14" x14ac:dyDescent="0.4">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A91" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>43827</v>
       </c>
       <c r="N91">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="92" spans="1:14" x14ac:dyDescent="0.4">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A92" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>43828</v>
       </c>
       <c r="N92">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="93" spans="1:14" x14ac:dyDescent="0.4">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A93" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>43829</v>
       </c>
       <c r="N93">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="94" spans="1:14" x14ac:dyDescent="0.4">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A94" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>43830</v>
       </c>
       <c r="N94">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="95" spans="1:14" x14ac:dyDescent="0.4">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A95" s="1"/>
     </row>
-    <row r="96" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="96" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A96" s="1"/>
     </row>
-    <row r="97" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="97" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A97" s="1"/>
     </row>
   </sheetData>
@@ -1533,19 +1569,19 @@
       <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="18.69140625" defaultRowHeight="34.200000000000003" customHeight="1" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultColWidth="18.7109375" defaultRowHeight="34.15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.53515625" style="2" customWidth="1"/>
+    <col min="1" max="1" width="12.5703125" style="2" customWidth="1"/>
     <col min="2" max="2" width="19" style="2" customWidth="1"/>
-    <col min="3" max="16384" width="18.69140625" style="2"/>
+    <col min="3" max="16384" width="18.7109375" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:10" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B1" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:10" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -1577,7 +1613,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:10" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>43739</v>
       </c>
@@ -1591,7 +1627,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:10" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <f>A3+1</f>
         <v>43740</v>
@@ -1606,553 +1642,553 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:10" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <f t="shared" ref="A5:A68" si="0">A4+1</f>
         <v>43741</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:10" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
         <f t="shared" si="0"/>
         <v>43742</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:10" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
         <f t="shared" si="0"/>
         <v>43743</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:10" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
         <f t="shared" si="0"/>
         <v>43744</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:10" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
         <f t="shared" si="0"/>
         <v>43745</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:10" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
         <f t="shared" si="0"/>
         <v>43746</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:10" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
         <f t="shared" si="0"/>
         <v>43747</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:10" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="3">
         <f t="shared" si="0"/>
         <v>43748</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:10" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="3">
         <f t="shared" si="0"/>
         <v>43749</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:10" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="3">
         <f t="shared" si="0"/>
         <v>43750</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:10" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="3">
         <f t="shared" si="0"/>
         <v>43751</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:10" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="3">
         <f t="shared" si="0"/>
         <v>43752</v>
       </c>
     </row>
-    <row r="17" spans="1:1" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:1" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="3">
         <f t="shared" si="0"/>
         <v>43753</v>
       </c>
     </row>
-    <row r="18" spans="1:1" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:1" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="3">
         <f t="shared" si="0"/>
         <v>43754</v>
       </c>
     </row>
-    <row r="19" spans="1:1" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:1" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="3">
         <f t="shared" si="0"/>
         <v>43755</v>
       </c>
     </row>
-    <row r="20" spans="1:1" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:1" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="3">
         <f t="shared" si="0"/>
         <v>43756</v>
       </c>
     </row>
-    <row r="21" spans="1:1" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:1" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="3">
         <f t="shared" si="0"/>
         <v>43757</v>
       </c>
     </row>
-    <row r="22" spans="1:1" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:1" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="3">
         <f t="shared" si="0"/>
         <v>43758</v>
       </c>
     </row>
-    <row r="23" spans="1:1" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:1" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="3">
         <f t="shared" si="0"/>
         <v>43759</v>
       </c>
     </row>
-    <row r="24" spans="1:1" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:1" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="3">
         <f t="shared" si="0"/>
         <v>43760</v>
       </c>
     </row>
-    <row r="25" spans="1:1" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:1" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="3">
         <f t="shared" si="0"/>
         <v>43761</v>
       </c>
     </row>
-    <row r="26" spans="1:1" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:1" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="3">
         <f t="shared" si="0"/>
         <v>43762</v>
       </c>
     </row>
-    <row r="27" spans="1:1" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:1" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="3">
         <f t="shared" si="0"/>
         <v>43763</v>
       </c>
     </row>
-    <row r="28" spans="1:1" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:1" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="3">
         <f t="shared" si="0"/>
         <v>43764</v>
       </c>
     </row>
-    <row r="29" spans="1:1" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:1" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="3">
         <f t="shared" si="0"/>
         <v>43765</v>
       </c>
     </row>
-    <row r="30" spans="1:1" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:1" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="3">
         <f t="shared" si="0"/>
         <v>43766</v>
       </c>
     </row>
-    <row r="31" spans="1:1" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:1" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="3">
         <f t="shared" si="0"/>
         <v>43767</v>
       </c>
     </row>
-    <row r="32" spans="1:1" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="32" spans="1:1" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="3">
         <f t="shared" si="0"/>
         <v>43768</v>
       </c>
     </row>
-    <row r="33" spans="1:1" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="33" spans="1:1" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="3">
         <f t="shared" si="0"/>
         <v>43769</v>
       </c>
     </row>
-    <row r="34" spans="1:1" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="34" spans="1:1" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="3">
         <f t="shared" si="0"/>
         <v>43770</v>
       </c>
     </row>
-    <row r="35" spans="1:1" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="35" spans="1:1" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="3">
         <f t="shared" si="0"/>
         <v>43771</v>
       </c>
     </row>
-    <row r="36" spans="1:1" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="36" spans="1:1" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="3">
         <f t="shared" si="0"/>
         <v>43772</v>
       </c>
     </row>
-    <row r="37" spans="1:1" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="37" spans="1:1" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="3">
         <f t="shared" si="0"/>
         <v>43773</v>
       </c>
     </row>
-    <row r="38" spans="1:1" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="38" spans="1:1" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="3">
         <f t="shared" si="0"/>
         <v>43774</v>
       </c>
     </row>
-    <row r="39" spans="1:1" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="39" spans="1:1" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="3">
         <f t="shared" si="0"/>
         <v>43775</v>
       </c>
     </row>
-    <row r="40" spans="1:1" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="40" spans="1:1" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="3">
         <f t="shared" si="0"/>
         <v>43776</v>
       </c>
     </row>
-    <row r="41" spans="1:1" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="41" spans="1:1" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="3">
         <f t="shared" si="0"/>
         <v>43777</v>
       </c>
     </row>
-    <row r="42" spans="1:1" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="42" spans="1:1" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="3">
         <f t="shared" si="0"/>
         <v>43778</v>
       </c>
     </row>
-    <row r="43" spans="1:1" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="43" spans="1:1" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="3">
         <f t="shared" si="0"/>
         <v>43779</v>
       </c>
     </row>
-    <row r="44" spans="1:1" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="44" spans="1:1" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="3">
         <f t="shared" si="0"/>
         <v>43780</v>
       </c>
     </row>
-    <row r="45" spans="1:1" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="45" spans="1:1" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="3">
         <f t="shared" si="0"/>
         <v>43781</v>
       </c>
     </row>
-    <row r="46" spans="1:1" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="46" spans="1:1" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="3">
         <f t="shared" si="0"/>
         <v>43782</v>
       </c>
     </row>
-    <row r="47" spans="1:1" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="47" spans="1:1" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="3">
         <f t="shared" si="0"/>
         <v>43783</v>
       </c>
     </row>
-    <row r="48" spans="1:1" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="48" spans="1:1" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="3">
         <f t="shared" si="0"/>
         <v>43784</v>
       </c>
     </row>
-    <row r="49" spans="1:1" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="49" spans="1:1" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="3">
         <f t="shared" si="0"/>
         <v>43785</v>
       </c>
     </row>
-    <row r="50" spans="1:1" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="50" spans="1:1" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="3">
         <f t="shared" si="0"/>
         <v>43786</v>
       </c>
     </row>
-    <row r="51" spans="1:1" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="51" spans="1:1" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="3">
         <f t="shared" si="0"/>
         <v>43787</v>
       </c>
     </row>
-    <row r="52" spans="1:1" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="52" spans="1:1" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="3">
         <f t="shared" si="0"/>
         <v>43788</v>
       </c>
     </row>
-    <row r="53" spans="1:1" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="53" spans="1:1" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="3">
         <f t="shared" si="0"/>
         <v>43789</v>
       </c>
     </row>
-    <row r="54" spans="1:1" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="54" spans="1:1" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="3">
         <f t="shared" si="0"/>
         <v>43790</v>
       </c>
     </row>
-    <row r="55" spans="1:1" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="55" spans="1:1" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="3">
         <f t="shared" si="0"/>
         <v>43791</v>
       </c>
     </row>
-    <row r="56" spans="1:1" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="56" spans="1:1" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="3">
         <f t="shared" si="0"/>
         <v>43792</v>
       </c>
     </row>
-    <row r="57" spans="1:1" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="57" spans="1:1" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="3">
         <f t="shared" si="0"/>
         <v>43793</v>
       </c>
     </row>
-    <row r="58" spans="1:1" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="58" spans="1:1" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="3">
         <f t="shared" si="0"/>
         <v>43794</v>
       </c>
     </row>
-    <row r="59" spans="1:1" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="59" spans="1:1" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="3">
         <f t="shared" si="0"/>
         <v>43795</v>
       </c>
     </row>
-    <row r="60" spans="1:1" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="60" spans="1:1" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="3">
         <f t="shared" si="0"/>
         <v>43796</v>
       </c>
     </row>
-    <row r="61" spans="1:1" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="61" spans="1:1" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="3">
         <f t="shared" si="0"/>
         <v>43797</v>
       </c>
     </row>
-    <row r="62" spans="1:1" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="62" spans="1:1" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="3">
         <f t="shared" si="0"/>
         <v>43798</v>
       </c>
     </row>
-    <row r="63" spans="1:1" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="63" spans="1:1" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="3">
         <f t="shared" si="0"/>
         <v>43799</v>
       </c>
     </row>
-    <row r="64" spans="1:1" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="64" spans="1:1" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="3">
         <f t="shared" si="0"/>
         <v>43800</v>
       </c>
     </row>
-    <row r="65" spans="1:1" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="65" spans="1:1" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="3">
         <f t="shared" si="0"/>
         <v>43801</v>
       </c>
     </row>
-    <row r="66" spans="1:1" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="66" spans="1:1" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" s="3">
         <f t="shared" si="0"/>
         <v>43802</v>
       </c>
     </row>
-    <row r="67" spans="1:1" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="67" spans="1:1" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" s="3">
         <f t="shared" si="0"/>
         <v>43803</v>
       </c>
     </row>
-    <row r="68" spans="1:1" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="68" spans="1:1" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="3">
         <f t="shared" si="0"/>
         <v>43804</v>
       </c>
     </row>
-    <row r="69" spans="1:1" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="69" spans="1:1" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" s="3">
         <f t="shared" ref="A69:A94" si="1">A68+1</f>
         <v>43805</v>
       </c>
     </row>
-    <row r="70" spans="1:1" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="70" spans="1:1" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" s="3">
         <f t="shared" si="1"/>
         <v>43806</v>
       </c>
     </row>
-    <row r="71" spans="1:1" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="71" spans="1:1" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" s="3">
         <f t="shared" si="1"/>
         <v>43807</v>
       </c>
     </row>
-    <row r="72" spans="1:1" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="72" spans="1:1" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" s="3">
         <f t="shared" si="1"/>
         <v>43808</v>
       </c>
     </row>
-    <row r="73" spans="1:1" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="73" spans="1:1" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" s="3">
         <f t="shared" si="1"/>
         <v>43809</v>
       </c>
     </row>
-    <row r="74" spans="1:1" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="74" spans="1:1" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" s="3">
         <f t="shared" si="1"/>
         <v>43810</v>
       </c>
     </row>
-    <row r="75" spans="1:1" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="75" spans="1:1" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" s="3">
         <f t="shared" si="1"/>
         <v>43811</v>
       </c>
     </row>
-    <row r="76" spans="1:1" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="76" spans="1:1" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76" s="3">
         <f t="shared" si="1"/>
         <v>43812</v>
       </c>
     </row>
-    <row r="77" spans="1:1" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="77" spans="1:1" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A77" s="3">
         <f t="shared" si="1"/>
         <v>43813</v>
       </c>
     </row>
-    <row r="78" spans="1:1" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="78" spans="1:1" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A78" s="3">
         <f t="shared" si="1"/>
         <v>43814</v>
       </c>
     </row>
-    <row r="79" spans="1:1" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="79" spans="1:1" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A79" s="3">
         <f t="shared" si="1"/>
         <v>43815</v>
       </c>
     </row>
-    <row r="80" spans="1:1" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="80" spans="1:1" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A80" s="3">
         <f t="shared" si="1"/>
         <v>43816</v>
       </c>
     </row>
-    <row r="81" spans="1:1" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="81" spans="1:1" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A81" s="3">
         <f t="shared" si="1"/>
         <v>43817</v>
       </c>
     </row>
-    <row r="82" spans="1:1" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="82" spans="1:1" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A82" s="3">
         <f t="shared" si="1"/>
         <v>43818</v>
       </c>
     </row>
-    <row r="83" spans="1:1" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="83" spans="1:1" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A83" s="3">
         <f t="shared" si="1"/>
         <v>43819</v>
       </c>
     </row>
-    <row r="84" spans="1:1" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="84" spans="1:1" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A84" s="3">
         <f t="shared" si="1"/>
         <v>43820</v>
       </c>
     </row>
-    <row r="85" spans="1:1" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="85" spans="1:1" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A85" s="3">
         <f t="shared" si="1"/>
         <v>43821</v>
       </c>
     </row>
-    <row r="86" spans="1:1" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="86" spans="1:1" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A86" s="3">
         <f t="shared" si="1"/>
         <v>43822</v>
       </c>
     </row>
-    <row r="87" spans="1:1" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="87" spans="1:1" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A87" s="3">
         <f t="shared" si="1"/>
         <v>43823</v>
       </c>
     </row>
-    <row r="88" spans="1:1" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="88" spans="1:1" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A88" s="3">
         <f t="shared" si="1"/>
         <v>43824</v>
       </c>
     </row>
-    <row r="89" spans="1:1" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="89" spans="1:1" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A89" s="3">
         <f t="shared" si="1"/>
         <v>43825</v>
       </c>
     </row>
-    <row r="90" spans="1:1" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="90" spans="1:1" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A90" s="3">
         <f t="shared" si="1"/>
         <v>43826</v>
       </c>
     </row>
-    <row r="91" spans="1:1" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="91" spans="1:1" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A91" s="3">
         <f t="shared" si="1"/>
         <v>43827</v>
       </c>
     </row>
-    <row r="92" spans="1:1" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="92" spans="1:1" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A92" s="3">
         <f t="shared" si="1"/>
         <v>43828</v>
       </c>
     </row>
-    <row r="93" spans="1:1" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="93" spans="1:1" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A93" s="3">
         <f t="shared" si="1"/>
         <v>43829</v>
       </c>
     </row>
-    <row r="94" spans="1:1" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="94" spans="1:1" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A94" s="3">
         <f t="shared" si="1"/>
         <v>43830</v>
       </c>
     </row>
-    <row r="95" spans="1:1" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="95" spans="1:1" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A95" s="3"/>
     </row>
-    <row r="96" spans="1:1" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="96" spans="1:1" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A96" s="3"/>
     </row>
-    <row r="97" spans="1:1" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="97" spans="1:1" ht="34.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A97" s="3"/>
     </row>
   </sheetData>
@@ -2166,7 +2202,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>